<commit_message>
script excel to tsv and handling empty fields
</commit_message>
<xml_diff>
--- a/src/resources/conclusies.xlsx
+++ b/src/resources/conclusies.xlsx
@@ -11,13 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
-  <si>
-    <t>conclusies</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -25,76 +19,37 @@
     <t>Conclusie</t>
   </si>
   <si>
+    <t>Informatie</t>
+  </si>
+  <si>
     <t>Image</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Conclusie 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>AVNRT</t>
   </si>
   <si>
-    <t>conclusie1-plaatje.jpeg</t>
+    <t>vraag1-plaatje.jpeg</t>
   </si>
   <si>
-    <t>Conclusie 2</t>
+    <t>Atriaal flutter/ atriaal tachycardie</t>
   </si>
   <si>
-    <t>conclusie2-plaatje.jpeg</t>
+    <t>B</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Conclusie 3
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>Atriaal tachycardie/ Atipische avnrt</t>
   </si>
   <si>
-    <t>conclusie3-plaatje.jpeg</t>
+    <t>AVRT/ AVNRT/ Atriaal tachycardie</t>
+  </si>
+  <si>
+    <t>A tachycardie / flutter/ multifocale</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>boezem fibrileren</t>
   </si>
 </sst>
 </file>
@@ -116,18 +71,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +101,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -168,6 +129,32 @@
       <bottom style="thin">
         <color indexed="11"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -207,12 +194,34 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -260,57 +269,151 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -332,6 +435,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
@@ -349,10 +454,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -529,11 +634,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -542,34 +650,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -817,12 +925,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1113,7 +1221,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1391,139 +1499,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:G9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.85156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.0547" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.5" style="1" customWidth="1"/>
-    <col min="6" max="7" width="8.35156" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" t="s" s="6">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" t="s" s="8">
+        <v>5</v>
+      </c>
+      <c r="E2" s="9"/>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+    <row r="3" ht="32.05" customHeight="1">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="11">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="9"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s" s="10">
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="D4" t="s" s="10">
+      <c r="B4" t="s" s="11">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="B5" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="9"/>
     </row>
-    <row r="5" ht="46.05" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="12">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s" s="13">
+    <row r="6" ht="32.05" customHeight="1">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="D5" t="s" s="10">
+      <c r="B6" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>5</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B7" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="9"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="12">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s" s="10">
-        <v>8</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="16"/>
     </row>
-    <row r="7" ht="323.5" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="12">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s" s="13">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+    <row r="9" ht="14.7" customHeight="1">
+      <c r="A9" s="17"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+    <row r="10" ht="14.7" customHeight="1">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>